<commit_message>
feat: Update data processing functions and add new input files for health data analysis
</commit_message>
<xml_diff>
--- a/data/inputs/orcamentos/sample_padrao1 - AG 0605 - 103481.xlsx
+++ b/data/inputs/orcamentos/sample_padrao1 - AG 0605 - 103481.xlsx
@@ -304,6 +304,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,7 +598,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>